<commit_message>
added response to an empty input
</commit_message>
<xml_diff>
--- a/Manual_Test.xlsx
+++ b/Manual_Test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-20.04\home\nassy\bootcamp\python\terminal_app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18DC4B9D-B42F-4532-B677-E2B1C3104AAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6FF6CA8-BF03-446E-B542-2B62AB07BCFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="4230" windowWidth="29040" windowHeight="17640" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -10315,7 +10315,7 @@
       <c r="J6" s="17"/>
       <c r="K6" s="17"/>
     </row>
-    <row r="7" spans="1:11" ht="75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" ht="84.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="17"/>
       <c r="B7" s="17"/>
       <c r="C7" s="31" t="s">

</xml_diff>